<commit_message>
A long overdue commit to this repo.
</commit_message>
<xml_diff>
--- a/IntegralData/H2_MEKENA/Book2.xlsx
+++ b/IntegralData/H2_MEKENA/Book2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kowalski/Quantum/Chemistry/TEST_KK/H2/ccpVTZ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmetcalf/Dropbox/Quantum Embedding/Codes/Lithium_Downfolding/Qiskit Chem/Hamiltonian_Downfolding_IBM/IntegralData/H2_MEKENA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD379381-92FB-4D43-8412-7FAF90F76627}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C3FFFB-B34F-9849-B559-D7D2C868058C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{B02C642C-F7E2-C042-BA38-C9C0B7A3D82D}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{B02C642C-F7E2-C042-BA38-C9C0B7A3D82D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3254,8 +3254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689A5D96-8A77-3243-A1F2-C44578187000}">
   <dimension ref="A5:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="A6:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>